<commit_message>
moved antenna cost to linear model based on vendor quotes
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7570F7-E1E6-B24A-95E0-AEF13FAAC923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5946DD3-5406-EF45-9263-EEE40D66F930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
   <si>
     <t>Description</t>
   </si>
@@ -737,9 +737,6 @@
     <t>commissioning_new</t>
   </si>
   <si>
-    <t>antenna_cost_factor</t>
-  </si>
-  <si>
     <t>exponent to apply to costs for larger dishes</t>
   </si>
   <si>
@@ -800,12 +797,6 @@
     <t>From quote for 3.5</t>
   </si>
   <si>
-    <t>C in the cost equation C+ kd^2.7</t>
-  </si>
-  <si>
-    <t>k in the cost equation</t>
-  </si>
-  <si>
     <t>antenna_cost_exponent</t>
   </si>
   <si>
@@ -897,6 +888,27 @@
   </si>
   <si>
     <t>Europe</t>
+  </si>
+  <si>
+    <t>antenna_cost_factor1</t>
+  </si>
+  <si>
+    <t>k1 in the cost equation</t>
+  </si>
+  <si>
+    <t>k2 in the cost equation</t>
+  </si>
+  <si>
+    <t>antenna_cost_factor2</t>
+  </si>
+  <si>
+    <t>Using a cost model fitting a quote for 3.5m + 12m ALMA dishes, we get cost = $1.3M + 8500*d^2.7</t>
+  </si>
+  <si>
+    <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-3M + $1.25M*d (no exponent term)</t>
+  </si>
+  <si>
+    <t>C in the cost equation C + k1d + k2d^2.7</t>
   </si>
 </sst>
 </file>
@@ -1412,36 +1424,36 @@
         <v>23</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>122</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34">
       <c r="A2" s="31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>0</v>
@@ -1626,36 +1638,36 @@
         <v>22</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17">
       <c r="A2" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1690,7 +1702,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C3" s="6">
         <v>6000000</v>
@@ -1723,7 +1735,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1758,7 +1770,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1798,10 +1810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
@@ -1849,7 +1861,7 @@
         <v>600000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34">
@@ -1874,12 +1886,12 @@
         <v>800000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>77</v>
@@ -1889,234 +1901,252 @@
         <v>885000</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="28">
         <f>1500000*1.18</f>
         <v>1770000</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C8" s="28">
         <f>1250000*1.18</f>
         <v>1475000</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="C9" s="28">
-        <v>1300000</v>
+        <v>-3000000</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="17">
       <c r="A10" s="12" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C10" s="29">
-        <v>8500</v>
-      </c>
-      <c r="D10" s="13"/>
+        <v>1250000</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="34">
+    <row r="11" spans="1:6" ht="17">
       <c r="A11" s="12" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="14">
-        <v>2.7</v>
-      </c>
-      <c r="D11" s="13"/>
+        <v>141</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="17">
+    <row r="12" spans="1:6" ht="34">
       <c r="A12" s="12" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="29">
-        <v>1500000</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>78</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="17">
       <c r="A13" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="30">
-        <v>2</v>
+        <v>89</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="29">
+        <v>1500000</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="17">
       <c r="A14" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="29">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="30">
+        <v>2</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="17">
       <c r="A15" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>116</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B15" s="12"/>
       <c r="C15" s="29">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" ht="51">
+    <row r="16" spans="1:6" ht="17">
       <c r="A16" s="12" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="C16" s="29">
+        <v>300000</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" ht="34">
+    <row r="17" spans="1:6" ht="51">
       <c r="A17" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C17" s="14">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="14">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="17">
+    <row r="19" spans="1:6" ht="34">
       <c r="A19" s="12" t="s">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="14">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="17">
       <c r="A20" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" ht="17">
       <c r="A21" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C21" s="14">
-        <v>1.4</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" ht="17">
+      <c r="A22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1.4</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2145,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>
@@ -2168,10 +2198,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="19">
         <v>250000</v>
@@ -2199,10 +2229,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="19">
         <v>250000</v>
@@ -2230,10 +2260,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="19">
         <f t="shared" ref="C4:I4" si="0">C2/2</f>
@@ -2274,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2291,10 +2321,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>
@@ -2314,7 +2344,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>40</v>
@@ -2343,10 +2373,10 @@
     </row>
     <row r="3" spans="1:9" ht="17">
       <c r="A3" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>101</v>
       </c>
       <c r="C3" s="19">
         <v>300</v>
@@ -2380,7 +2410,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
updated cost numbers from updated vendo quotes
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5946DD3-5406-EF45-9263-EEE40D66F930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62203C68-C75A-0D4F-B2A6-EC18E80D24BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
@@ -1941,8 +1941,8 @@
       <c r="B9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="28">
-        <v>-3000000</v>
+      <c r="C9" s="29">
+        <v>-4050000</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -1954,7 +1954,7 @@
         <v>140</v>
       </c>
       <c r="C10" s="29">
-        <v>1250000</v>
+        <v>1687500</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
added ability to leave sites out of backend upgrades, added cost example for srr
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62203C68-C75A-0D4F-B2A6-EC18E80D24BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F274E3B-C2E9-8749-95D6-0F415DB978E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,9 +779,6 @@
     <t>Cost for first prototype</t>
   </si>
   <si>
-    <t>From quote</t>
-  </si>
-  <si>
     <t>antenna_development_nre</t>
   </si>
   <si>
@@ -809,9 +806,6 @@
     <t>From Astro2020 paper</t>
   </si>
   <si>
-    <t>maser_cost</t>
-  </si>
-  <si>
     <t>Maser</t>
   </si>
   <si>
@@ -909,6 +903,12 @@
   </si>
   <si>
     <t>C in the cost equation C + k1d + k2d^2.7</t>
+  </si>
+  <si>
+    <t>from "station cost estimate" sheet (Kari)</t>
+  </si>
+  <si>
+    <t>timing_dbe_cost</t>
   </si>
 </sst>
 </file>
@@ -1424,36 +1424,36 @@
         <v>23</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="E1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>120</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34">
       <c r="A2" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>0</v>
@@ -1638,36 +1638,36 @@
         <v>22</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17">
       <c r="A2" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" s="6">
         <v>6000000</v>
@@ -1735,7 +1735,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1770,7 +1770,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
@@ -1861,7 +1861,7 @@
         <v>600000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34">
@@ -1886,12 +1886,12 @@
         <v>800000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>77</v>
@@ -1901,12 +1901,12 @@
         <v>885000</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>101</v>
@@ -1916,30 +1916,30 @@
         <v>1770000</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="28">
         <f>1250000*1.18</f>
         <v>1475000</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C9" s="29">
         <v>-4050000</v>
@@ -1948,39 +1948,39 @@
     </row>
     <row r="10" spans="1:6" ht="17">
       <c r="A10" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" s="29">
         <v>1687500</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="29">
         <v>0</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="34">
       <c r="A12" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>88</v>
@@ -1997,13 +1997,13 @@
         <v>89</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="29">
-        <v>1500000</v>
+        <v>1300000</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -2040,23 +2040,23 @@
     </row>
     <row r="16" spans="1:6" ht="17">
       <c r="A16" s="12" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" s="29">
-        <v>300000</v>
+        <v>850000</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="51">
       <c r="A17" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>15</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>9</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="19" spans="1:6" ht="34">
       <c r="A19" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>10</v>
@@ -2175,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>
@@ -2321,10 +2321,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
updated calculation of NRE
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F274E3B-C2E9-8749-95D6-0F415DB978E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F16C0E-DD37-F549-800A-F9B9D5CE1C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
   <si>
     <t>Description</t>
   </si>
@@ -704,9 +704,6 @@
     <t>Compute Cost / PB</t>
   </si>
   <si>
-    <t>NRE for 3.5m Antenna</t>
-  </si>
-  <si>
     <t>guess to match quote</t>
   </si>
   <si>
@@ -776,24 +773,9 @@
     <t>Costs per day of trip</t>
   </si>
   <si>
-    <t>Cost for first prototype</t>
-  </si>
-  <si>
     <t>antenna_development_nre</t>
   </si>
   <si>
-    <t>antenna_prototype</t>
-  </si>
-  <si>
-    <t>antenna_multiple</t>
-  </si>
-  <si>
-    <t>Cost for additional units</t>
-  </si>
-  <si>
-    <t>From quote for 3.5</t>
-  </si>
-  <si>
     <t>antenna_cost_exponent</t>
   </si>
   <si>
@@ -899,9 +881,6 @@
     <t>Using a cost model fitting a quote for 3.5m + 12m ALMA dishes, we get cost = $1.3M + 8500*d^2.7</t>
   </si>
   <si>
-    <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-3M + $1.25M*d (no exponent term)</t>
-  </si>
-  <si>
     <t>C in the cost equation C + k1d + k2d^2.7</t>
   </si>
   <si>
@@ -909,6 +888,12 @@
   </si>
   <si>
     <t>timing_dbe_cost</t>
+  </si>
+  <si>
+    <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-4M + $1.687M*d (no exponent term)</t>
+  </si>
+  <si>
+    <t>Multiple of antenna cost for NRE + proto</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196B2738-0FDD-4912-B5C0-AAFA06FDBC1C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1424,36 +1409,36 @@
         <v>23</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34">
       <c r="A2" s="31" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>0</v>
@@ -1638,36 +1623,36 @@
         <v>22</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17">
       <c r="A2" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1702,7 +1687,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C3" s="6">
         <v>6000000</v>
@@ -1735,7 +1720,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1770,7 +1755,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1810,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
@@ -1841,10 +1826,10 @@
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="21">
         <v>250000</v>
@@ -1852,24 +1837,24 @@
     </row>
     <row r="3" spans="1:6" ht="51">
       <c r="A3" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="21">
         <v>600000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34">
       <c r="A4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="21">
         <v>100000</v>
@@ -1877,276 +1862,243 @@
     </row>
     <row r="5" spans="1:6" ht="34">
       <c r="A5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="22">
         <v>800000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="C6" s="28">
-        <f>750000*1.18</f>
-        <v>885000</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>106</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="28">
-        <f>1500000*1.18</f>
-        <v>1770000</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>106</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C7" s="29">
+        <v>-4050000</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="28">
-        <f>1250000*1.18</f>
-        <v>1475000</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>106</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="29">
+        <v>1687500</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="29">
-        <v>-4050000</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="17">
+        <v>134</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" ht="34">
       <c r="A10" s="12" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="29">
-        <v>1687500</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>141</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="12" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="C11" s="29">
-        <v>0</v>
+        <v>1300000</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="34">
+    <row r="12" spans="1:6" ht="17">
       <c r="A12" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="14">
-        <v>2.7</v>
-      </c>
-      <c r="D12" s="13"/>
+        <v>89</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="30">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="17">
       <c r="A13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>109</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B13" s="12"/>
       <c r="C13" s="29">
-        <v>1300000</v>
+        <v>0</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="17">
       <c r="A14" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="30">
-        <v>2</v>
+        <v>138</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="29">
+        <v>850000</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="17">
+    <row r="15" spans="1:6" ht="51">
       <c r="A15" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="29">
-        <v>0</v>
+        <v>126</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" ht="17">
+    <row r="16" spans="1:6" ht="34">
       <c r="A16" s="12" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="29">
-        <v>850000</v>
+        <v>9</v>
+      </c>
+      <c r="C16" s="14">
+        <v>2.5</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" ht="51">
+    <row r="17" spans="1:6" ht="34">
       <c r="A17" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" s="14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" ht="34">
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" s="12" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C18" s="14">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="34">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" s="12" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19" s="14">
-        <v>10</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>20</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="17">
       <c r="A20" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C20" s="14">
-        <v>25</v>
+        <v>1.4</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="17">
-      <c r="A21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" ht="17">
-      <c r="A22" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1.4</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2175,10 +2127,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>
@@ -2198,10 +2150,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="19">
         <v>250000</v>
@@ -2229,10 +2181,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="19">
         <v>250000</v>
@@ -2260,10 +2212,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="19">
         <f t="shared" ref="C4:I4" si="0">C2/2</f>
@@ -2321,10 +2273,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>29</v>
@@ -2344,7 +2296,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>40</v>
@@ -2373,10 +2325,10 @@
     </row>
     <row r="3" spans="1:9" ht="17">
       <c r="A3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="C3" s="19">
         <v>300</v>

</xml_diff>

<commit_message>
updated media costs and cleaned up spreadsheet
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F16C0E-DD37-F549-800A-F9B9D5CE1C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71DA19D-8207-BE4F-987B-03D50D2DBE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="27400" windowHeight="17500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="760" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="153">
   <si>
     <t>Description</t>
   </si>
@@ -671,12 +671,6 @@
     <t>Max number of nights of data to own. If we have 7, that means we can record 7 nights worth before needing to recycle. Need to dump it somewhere else in that time.</t>
   </si>
   <si>
-    <t>Based on hard disks?</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -894,6 +888,48 @@
   </si>
   <si>
     <t>Multiple of antenna cost for NRE + proto</t>
+  </si>
+  <si>
+    <t>Based on 15.36 TB NVME SSD are e.g. $3,870 each: https://www.cdw.com/product/micron-9300-pro-ssd-15.36-tb-u.2-pcie-nvme/5529945</t>
+  </si>
+  <si>
+    <t>bandwidth</t>
+  </si>
+  <si>
+    <t>bit_depth</t>
+  </si>
+  <si>
+    <t>sidebands</t>
+  </si>
+  <si>
+    <t>polarizations</t>
+  </si>
+  <si>
+    <t>frequencies</t>
+  </si>
+  <si>
+    <t>oversampling</t>
+  </si>
+  <si>
+    <t>recording_hours_per_ay</t>
+  </si>
+  <si>
+    <t>holding_months</t>
+  </si>
+  <si>
+    <t>processing_months</t>
+  </si>
+  <si>
+    <t>media_cost_pb</t>
+  </si>
+  <si>
+    <t>recorder_cost</t>
+  </si>
+  <si>
+    <t>media_on_hand</t>
+  </si>
+  <si>
+    <t>fte_cost</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1041,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1016,7 +1052,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1072,6 +1107,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1392,207 +1429,207 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196B2738-0FDD-4912-B5C0-AAFA06FDBC1C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="31" customWidth="1"/>
-    <col min="3" max="10" width="24.5703125" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="31"/>
+    <col min="1" max="1" width="21.5703125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="30" customWidth="1"/>
+    <col min="3" max="10" width="24.5703125" style="30" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="2" spans="1:10" ht="34">
-      <c r="A2" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>1</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>2</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="30">
         <v>2</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="30">
         <v>2</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <v>2</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="30">
         <v>2.5</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="34">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>1</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>2</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>2</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>0.5</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <v>0.5</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>2</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="30">
         <v>2.5</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="30">
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="51">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>0</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>3</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>1</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>0.5</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <v>0.5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>2</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <v>2.5</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>0</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>3</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>0</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>0</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <v>0</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>5</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="30">
         <v>0</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="30">
         <v>10</v>
       </c>
     </row>
@@ -1619,66 +1656,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="17">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>106</v>
+      <c r="B1" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17">
-      <c r="A2" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1687,7 +1724,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" s="6">
         <v>6000000</v>
@@ -1720,7 +1757,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1755,9 +1792,9 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="27">
+        <v>115</v>
+      </c>
+      <c r="C5" s="26">
         <v>0</v>
       </c>
       <c r="D5" s="6">
@@ -1803,302 +1840,302 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="24" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="20">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51">
+      <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="20">
+        <v>600000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34">
+      <c r="A4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="20">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34">
+      <c r="A5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="21">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="51">
-      <c r="A3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="21">
-        <v>600000</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="34">
-      <c r="A4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="21">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34">
-      <c r="A5" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>800000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="27">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="17">
+      <c r="A7" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="28">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="17">
-      <c r="A7" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="29">
+        <v>134</v>
+      </c>
+      <c r="C7" s="28">
         <v>-4050000</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="17">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="28">
+        <v>1687500</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="29">
-        <v>1687500</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="17">
-      <c r="A9" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>133</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="D9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="34">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="13">
+        <v>2.7</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="17">
+      <c r="A11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C11" s="28">
+        <v>1300000</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="17">
+      <c r="A12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="14">
-        <v>2.7</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="12" t="s">
+      <c r="B12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="29">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="17">
+      <c r="A13" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="17">
+      <c r="A14" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="29">
-        <v>1300000</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="30">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="17">
-      <c r="A13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="29">
-        <v>0</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>850000</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="D14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" ht="51">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="34">
+      <c r="A16" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="34">
+      <c r="A17" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="14">
+      <c r="B17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="13">
+        <v>10</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="17">
+      <c r="A18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="13">
+        <v>25</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="17">
+      <c r="A19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="34">
-      <c r="A16" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="34">
-      <c r="A17" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="14">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="17">
-      <c r="A18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="14">
-        <v>25</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="17">
-      <c r="A19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="17">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>1.4</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2122,126 +2159,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="A2" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="18">
         <v>250000</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="18">
         <v>250000</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="18">
         <v>175000</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="18">
         <v>150000</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="18">
         <v>150000</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="18">
         <f>C2</f>
         <v>250000</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="18">
         <f>C2*1.5</f>
         <v>375000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="A3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="18">
         <v>250000</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>250000</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>175000</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="18">
         <v>150000</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="18">
         <v>150000</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="18">
         <f>C3</f>
         <v>250000</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <f>C3*1.5</f>
         <v>375000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="A4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="18">
         <f t="shared" ref="C4:I4" si="0">C2/2</f>
         <v>125000</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <f t="shared" ref="D4" si="1">D2/2</f>
         <v>125000</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <f t="shared" si="0"/>
         <v>87500</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <f t="shared" si="0"/>
         <v>125000</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <f t="shared" si="0"/>
         <v>187500</v>
       </c>
@@ -2268,87 +2305,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1500</v>
+      </c>
+      <c r="D2" s="18">
+        <v>1500</v>
+      </c>
+      <c r="E2" s="18">
+        <v>4000</v>
+      </c>
+      <c r="F2" s="18">
+        <v>6000</v>
+      </c>
+      <c r="G2" s="18">
+        <v>6000</v>
+      </c>
+      <c r="H2" s="18">
+        <v>8000</v>
+      </c>
+      <c r="I2" s="18">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17">
+      <c r="A3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="19">
-        <v>1500</v>
-      </c>
-      <c r="D2" s="19">
-        <v>1500</v>
-      </c>
-      <c r="E2" s="19">
-        <v>4000</v>
-      </c>
-      <c r="F2" s="19">
-        <v>6000</v>
-      </c>
-      <c r="G2" s="19">
-        <v>6000</v>
-      </c>
-      <c r="H2" s="19">
-        <v>8000</v>
-      </c>
-      <c r="I2" s="19">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17">
-      <c r="A3" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>300</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>300</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>200</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="18">
         <v>200</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="18">
         <v>200</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="18">
         <v>300</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>2000</v>
       </c>
     </row>
@@ -2359,162 +2396,205 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06B76BD-0759-4FEE-B338-554318A1054B}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="32" customFormat="1">
+      <c r="A1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="3">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4">
+        <v>266000</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="5">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="C14" s="25">
+        <v>125000</v>
+      </c>
+      <c r="D14" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="4">
-        <v>100000</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="4">
-        <v>30000</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="5">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="26">
-        <v>125000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cost model with better dbe cost calculations
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71DA19D-8207-BE4F-987B-03D50D2DBE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCB7647-B2DF-8149-AF09-09C8820838F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="760" windowWidth="27400" windowHeight="17500" tabRatio="860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="760" windowWidth="32880" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
   <si>
     <t>Description</t>
   </si>
@@ -782,9 +782,6 @@
     <t>From Astro2020 paper</t>
   </si>
   <si>
-    <t>Maser</t>
-  </si>
-  <si>
     <t>xx</t>
   </si>
   <si>
@@ -881,9 +878,6 @@
     <t>from "station cost estimate" sheet (Kari)</t>
   </si>
   <si>
-    <t>timing_dbe_cost</t>
-  </si>
-  <si>
     <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-4M + $1.687M*d (no exponent term)</t>
   </si>
   <si>
@@ -930,6 +924,24 @@
   </si>
   <si>
     <t>fte_cost</t>
+  </si>
+  <si>
+    <t>maser_cost</t>
+  </si>
+  <si>
+    <t>Cost for maser &amp; components</t>
+  </si>
+  <si>
+    <t>from Jono</t>
+  </si>
+  <si>
+    <t>dbe_cost</t>
+  </si>
+  <si>
+    <t>Cost for BDC &amp; DBE</t>
+  </si>
+  <si>
+    <t>from Ranjani - assumes 2SB, 2pol</t>
   </si>
 </sst>
 </file>
@@ -942,7 +954,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1433,7 +1445,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="30" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="30" customWidth="1"/>
@@ -1441,41 +1453,41 @@
     <col min="11" max="16384" width="8.7109375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34">
+    </row>
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>0</v>
@@ -1505,7 +1517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34">
+    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
@@ -1569,7 +1581,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="51">
+    <row r="5" spans="1:10" ht="54" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -1601,7 +1613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34">
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1658,7 @@
       <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="3" customWidth="1"/>
@@ -1655,41 +1667,41 @@
     <col min="7" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="17">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17">
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>0</v>
@@ -1719,12 +1731,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="6">
         <v>6000000</v>
@@ -1752,12 +1764,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1787,12 +1799,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="26">
         <v>0</v>
@@ -1832,13 +1844,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.28515625" style="24" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="24" customWidth="1"/>
@@ -1847,7 +1859,7 @@
     <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -1872,7 +1884,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51">
+    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34">
+    <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>83</v>
       </c>
@@ -1897,7 +1909,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34">
+    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>84</v>
       </c>
@@ -1911,63 +1923,63 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" s="27">
         <v>2</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="28">
         <v>-4050000</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="C8" s="28">
         <v>1687500</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="17">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="34">
+    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>99</v>
       </c>
@@ -1981,7 +1993,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="17">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>86</v>
       </c>
@@ -1992,12 +2004,12 @@
         <v>1300000</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="17">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>87</v>
       </c>
@@ -2013,7 +2025,7 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="17">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>88</v>
       </c>
@@ -2027,115 +2039,131 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="17">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="C14" s="28">
-        <v>850000</v>
+        <v>500000</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="51">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="C15" s="28">
+        <v>250000</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="34">
+    <row r="16" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C16" s="13">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="34">
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="13">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" ht="17">
+    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="17">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C19" s="13">
-        <v>1</v>
-      </c>
-      <c r="D19" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" ht="17">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C20" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,23 +2179,23 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="3" customWidth="1"/>
     <col min="5" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>29</v>
@@ -2185,7 +2213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>89</v>
       </c>
@@ -2216,7 +2244,7 @@
         <v>375000</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>90</v>
       </c>
@@ -2247,7 +2275,7 @@
         <v>375000</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>91</v>
       </c>
@@ -2297,23 +2325,23 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34">
+    <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>29</v>
@@ -2331,7 +2359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>95</v>
       </c>
@@ -2360,7 +2388,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>96</v>
       </c>
@@ -2398,18 +2426,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06B76BD-0759-4FEE-B338-554318A1054B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="32" customFormat="1">
+    <row r="1" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
@@ -2423,9 +2451,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>68</v>
@@ -2437,9 +2465,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -2451,9 +2479,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>43</v>
@@ -2465,9 +2493,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>45</v>
@@ -2479,9 +2507,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>70</v>
@@ -2493,9 +2521,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>48</v>
@@ -2507,9 +2535,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2519,9 +2547,9 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>57</v>
@@ -2531,9 +2559,9 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>56</v>
@@ -2543,9 +2571,9 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -2554,12 +2582,12 @@
         <v>266000</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>55</v>
@@ -2569,9 +2597,9 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2583,9 +2611,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
added transportation cost for new antennas
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCB7647-B2DF-8149-AF09-09C8820838F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AACE54-BC07-8344-97BC-0613A0DDE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="760" windowWidth="32880" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="160">
   <si>
     <t>Description</t>
   </si>
@@ -942,6 +942,15 @@
   </si>
   <si>
     <t>from Ranjani - assumes 2SB, 2pol</t>
+  </si>
+  <si>
+    <t>antenna_transport_cost</t>
+  </si>
+  <si>
+    <t>Cost to move antenna from mfg to site</t>
+  </si>
+  <si>
+    <t>from Bragg Crane quotes - about $150k land voyage + $250k sea voyage</t>
   </si>
 </sst>
 </file>
@@ -1844,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2071,99 +2080,115 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="13">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="C16" s="28">
+        <v>400000</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>18</v>
+        <v>159</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C17" s="13">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="13">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C20" s="13">
-        <v>1</v>
-      </c>
-      <c r="D20" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C21" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moved NRE out of capital costs
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AACE54-BC07-8344-97BC-0613A0DDE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5EFBD1-24CA-A748-AFB5-75380832A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="760" windowWidth="32880" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="161">
   <si>
     <t>Description</t>
   </si>
@@ -881,9 +881,6 @@
     <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-4M + $1.687M*d (no exponent term)</t>
   </si>
   <si>
-    <t>Multiple of antenna cost for NRE + proto</t>
-  </si>
-  <si>
     <t>Based on 15.36 TB NVME SSD are e.g. $3,870 each: https://www.cdw.com/product/micron-9300-pro-ssd-15.36-tb-u.2-pcie-nvme/5529945</t>
   </si>
   <si>
@@ -951,6 +948,12 @@
   </si>
   <si>
     <t>from Bragg Crane quotes - about $150k land voyage + $250k sea voyage</t>
+  </si>
+  <si>
+    <t>Flat NRE cost for design work</t>
+  </si>
+  <si>
+    <t>Seems reasonable from vendor quotes</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1065,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1130,6 +1133,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1856,7 +1860,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1937,12 +1941,14 @@
         <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C6" s="27">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>2000000</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -2050,48 +2056,48 @@
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="C14" s="28">
         <v>500000</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="C15" s="28">
         <v>250000</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="C16" s="28">
         <v>400000</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -2478,7 +2484,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>68</v>
@@ -2492,7 +2498,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -2506,7 +2512,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>43</v>
@@ -2520,7 +2526,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>45</v>
@@ -2534,7 +2540,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>70</v>
@@ -2548,7 +2554,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>48</v>
@@ -2562,7 +2568,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2574,7 +2580,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>57</v>
@@ -2586,7 +2592,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>56</v>
@@ -2598,7 +2604,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -2607,12 +2613,12 @@
         <v>266000</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>55</v>
@@ -2624,7 +2630,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2638,7 +2644,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
added group support equipment for new sites
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5EFBD1-24CA-A748-AFB5-75380832A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE9CB24-9174-3049-AF09-5D7325CBCF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="760" windowWidth="32880" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="27100" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="163">
   <si>
     <t>Description</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>Seems reasonable from vendor quotes</t>
+  </si>
+  <si>
+    <t>ground_support_equipment</t>
+  </si>
+  <si>
+    <t>equipment needed for testing, etc.</t>
   </si>
 </sst>
 </file>
@@ -1857,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1911,12 +1917,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
       <c r="C4" s="20">
         <v>100000</v>
@@ -1924,277 +1930,288 @@
     </row>
     <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="20">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C6" s="21">
         <v>800000</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="27">
-        <v>2000000</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="28">
-        <v>-4050000</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="C7" s="27">
+        <v>2000000</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>129</v>
+        <v>100</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="C8" s="28">
-        <v>1687500</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+        <v>-4050000</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1687500</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="13">
-        <v>2.7</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="28">
-        <v>1300000</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>134</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C11" s="13">
+        <v>2.7</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="29">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1300000</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="28">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="29">
+        <v>2</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>151</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="28">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C15" s="28">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C16" s="28">
-        <v>400000</v>
+        <v>250000</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="13">
-        <v>1</v>
+        <v>157</v>
+      </c>
+      <c r="C17" s="28">
+        <v>400000</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>18</v>
+        <v>158</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C18" s="13">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="13">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C21" s="13">
-        <v>1</v>
-      </c>
-      <c r="D21" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C22" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added site rental for non-owned sites, per night of observation
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE9CB24-9174-3049-AF09-5D7325CBCF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F4CB4B-41EE-4545-AF47-5982D32068FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="27100" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="166">
   <si>
     <t>Description</t>
   </si>
@@ -960,6 +960,15 @@
   </si>
   <si>
     <t>equipment needed for testing, etc.</t>
+  </si>
+  <si>
+    <t>existing_site_rental_per_night</t>
+  </si>
+  <si>
+    <t>Cost to use a telescope per night if we don't own it</t>
+  </si>
+  <si>
+    <t>This is what it costs for a block of time from SMA?</t>
   </si>
 </sst>
 </file>
@@ -1863,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2119,99 +2128,115 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C18" s="28">
+        <v>10000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="54" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C19" s="13">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="13">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C22" s="13">
-        <v>1</v>
-      </c>
-      <c r="D22" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C23" s="13">
-        <v>1.4</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
now adding a little cost for spare parts for backend and recorder
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F4CB4B-41EE-4545-AF47-5982D32068FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3B7618-5A18-934D-B2F0-96324EDADF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="27100" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -981,7 +981,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1049,6 +1049,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1080,7 +1086,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1149,6 +1155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1875,7 +1882,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2087,8 +2094,8 @@
       <c r="B15" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="28">
-        <v>500000</v>
+      <c r="C15" s="34">
+        <v>632000</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>152</v>
@@ -2500,7 +2507,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2673,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="4">
-        <v>30000</v>
+        <v>45000</v>
       </c>
       <c r="D12" s="3"/>
     </row>

</xml_diff>

<commit_message>
preparing for pypi release
</commit_message>
<xml_diff>
--- a/ngehtutil/cost/cost_constants.xlsx
+++ b/ngehtutil/cost/cost_constants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoppenheimer/src/ngeht-util/ngehtutil/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3B7618-5A18-934D-B2F0-96324EDADF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79790886-6C46-7241-940B-6DCC848B119A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="27100" windowHeight="17500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="27100" windowHeight="17500" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonomyModeValues" sheetId="21" r:id="rId1"/>
@@ -207,7 +207,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -216,12 +216,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-$50 per set of 8 SSD, 32 SSD per 3PB array, two-way shipping (per Lindy estimate)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$50 per set of 8 SSD, 32 SSD per 3PB array, two-way shipping (per Lindy estimate)</t>
         </r>
       </text>
     </comment>
@@ -328,7 +337,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -337,12 +346,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-No charge to transfer between tiers</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>No charge to transfer between tiers</t>
         </r>
       </text>
     </comment>
@@ -376,21 +394,21 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Aaron Oppenheimer:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Per Lindy? This is PER PB</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Aaron Oppenheimer
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is PER PB</t>
         </r>
       </text>
     </comment>
@@ -400,7 +418,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -409,12 +427,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-$0.20/GB/mo</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$0.20/GB/mo</t>
         </r>
       </text>
     </comment>
@@ -424,7 +451,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -433,12 +460,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-$0.012/GB/mo</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$0.012/GB/mo</t>
         </r>
       </text>
     </comment>
@@ -448,7 +484,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -457,12 +493,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-$0.05GB to transfer from archive to active storage</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$0.05GB to transfer from archive to active storage</t>
         </r>
       </text>
     </comment>
@@ -869,15 +914,9 @@
     <t>antenna_cost_factor2</t>
   </si>
   <si>
-    <t>Using a cost model fitting a quote for 3.5m + 12m ALMA dishes, we get cost = $1.3M + 8500*d^2.7</t>
-  </si>
-  <si>
     <t>C in the cost equation C + k1d + k2d^2.7</t>
   </si>
   <si>
-    <t>from "station cost estimate" sheet (Kari)</t>
-  </si>
-  <si>
     <t>Using a cost model fitting quotes for 3.5, 6, and 10, we get cost = $-4M + $1.687M*d (no exponent term)</t>
   </si>
   <si>
@@ -929,27 +968,18 @@
     <t>Cost for maser &amp; components</t>
   </si>
   <si>
-    <t>from Jono</t>
-  </si>
-  <si>
     <t>dbe_cost</t>
   </si>
   <si>
     <t>Cost for BDC &amp; DBE</t>
   </si>
   <si>
-    <t>from Ranjani - assumes 2SB, 2pol</t>
-  </si>
-  <si>
     <t>antenna_transport_cost</t>
   </si>
   <si>
     <t>Cost to move antenna from mfg to site</t>
   </si>
   <si>
-    <t>from Bragg Crane quotes - about $150k land voyage + $250k sea voyage</t>
-  </si>
-  <si>
     <t>Flat NRE cost for design work</t>
   </si>
   <si>
@@ -968,7 +998,22 @@
     <t>Cost to use a telescope per night if we don't own it</t>
   </si>
   <si>
-    <t>This is what it costs for a block of time from SMA?</t>
+    <t>Recent inquires</t>
+  </si>
+  <si>
+    <t>Assumes 2SB, 2pol</t>
+  </si>
+  <si>
+    <t>From quotes - About $150k land voyage + $250k sea voyage</t>
+  </si>
+  <si>
+    <t>In cases where we're not just doing on-off observations that falls under a site's usual mandate</t>
+  </si>
+  <si>
+    <t>Using a cost model fitting a quote for 3.5m + 12m, we get cost = $1.3M + 8500*d^2.7</t>
+  </si>
+  <si>
+    <t>from "station cost estimate" sheet</t>
   </si>
 </sst>
 </file>
@@ -1689,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254F840D-40C8-4F0A-A5D4-57C338ABE3A6}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1881,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E026190B-EC10-4D4E-AB68-769C755BB90E}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1935,10 +1980,10 @@
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C4" s="20">
         <v>100000</v>
@@ -1974,13 +2019,13 @@
         <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C7" s="27">
         <v>2000000</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
@@ -1988,7 +2033,7 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="28">
         <v>-4050000</v>
@@ -2006,7 +2051,7 @@
         <v>1687500</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -2022,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2052,7 +2097,7 @@
         <v>1300000</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -2089,64 +2134,64 @@
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C15" s="34">
-        <v>632000</v>
+        <v>650000</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C16" s="28">
         <v>250000</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C17" s="28">
         <v>400000</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C18" s="28">
         <v>10000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -2533,7 +2578,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>68</v>
@@ -2547,7 +2592,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -2561,7 +2606,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>43</v>
@@ -2575,7 +2620,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>45</v>
@@ -2589,7 +2634,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>70</v>
@@ -2603,7 +2648,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>48</v>
@@ -2617,7 +2662,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2629,7 +2674,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>57</v>
@@ -2641,7 +2686,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>56</v>
@@ -2653,7 +2698,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -2662,12 +2707,12 @@
         <v>266000</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>55</v>
@@ -2679,7 +2724,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -2693,7 +2738,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
         <v>71</v>

</xml_diff>